<commit_message>
Global commit: - Add supplier list and change supplier - New UI - Full remake and refactoring code
</commit_message>
<xml_diff>
--- a/data/table/database.xlsx
+++ b/data/table/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Purchase_generator\data\table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Purchase_generator [V3]\data\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070357CC-A980-4FBC-8D5E-661C19EAB688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43B7555-40DA-4A1D-B93C-1F325186952E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30AF6E45-24C8-4B4E-A83D-5BACAC6596C8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="237">
   <si>
     <t>Артикул</t>
   </si>
@@ -741,6 +741,12 @@
   </si>
   <si>
     <t>KC-3059</t>
+  </si>
+  <si>
+    <t>Вася Пупкин</t>
+  </si>
+  <si>
+    <t>Иван Иванов</t>
   </si>
 </sst>
 </file>
@@ -1179,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDCFE40-2717-4B3A-BE28-34D738E90ACF}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2917,8 +2923,68 @@
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78"/>
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B78" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D78" s="1">
+        <v>777</v>
+      </c>
+      <c r="F78" s="6" t="str">
+        <f t="shared" ref="F78:F80" si="2">"images/"&amp;B78&amp;".jpg"</f>
+        <v>images/vl-king-ytyg-kc-3059.jpg</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B79" t="s">
+        <v>151</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D79" s="1">
+        <v>888</v>
+      </c>
+      <c r="F79" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>images/vl-king-ytyg-kc-3059.jpg</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B80" t="s">
+        <v>150</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F80" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>images/vl-king-ytyg-kc-3043.jpg</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>236</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">

</xml_diff>